<commit_message>
compiled requested columns in report-checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111O3ENTERPRISESRL/o3enterprise/ris/7.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111O3ENTERPRISESRL/o3enterprise/ris/7.0.0/report-checklist.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -110,7 +110,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>Obiettivo</t>
@@ -118,7 +117,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">: In questo foglio si riportano i pre requisiti/assunzioni necessari all'accreditamento del software dei </t>
@@ -127,7 +125,6 @@
       <rPr>
         <i/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>client</t>
@@ -135,7 +132,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve"> che ne hanno fatto richiesta, e utili alla compilazione della presente Checklist.</t>
@@ -161,7 +157,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">I file CDA2 necessari all'esecuzione dei test di accreditamento devono essere costruiti secondo le specifiche nazionali HL7 - http://www.hl7italia.it/hl7italia_D7/node/2359 e coerentemente ai casi di test descritti.</t>
@@ -280,6 +275,12 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
+    <t>5fbec3db2d98640e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50504.4.4.930de4356d88c2c4150942eac66d3ef84e9b237be1c5ed78390cc9e0426578ff.ddb5b5d86e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
     <t>SI</t>
   </si>
   <si>
@@ -324,7 +325,6 @@
         <b/>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Precondizioni:
@@ -333,7 +333,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Il fornitore utilizza un token jwt mancante di campi obbligatori, quindi non valido.
@@ -344,7 +343,6 @@
         <b/>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Descrizione di Business del caso di test: 
@@ -353,7 +351,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
@@ -375,7 +372,6 @@
         <b/>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Precondizioni:
@@ -384,7 +380,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Il fornitore utilizza un token jwt con dei campi valorizzati in maniera errata.
@@ -395,7 +390,6 @@
         <b/>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Descrizione di Business del caso di test: 
@@ -404,7 +398,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
@@ -419,6 +412,12 @@
 "ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", "GESTIONE ERRORE".</t>
   </si>
   <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'applicativo non comunica direttamente con il gateway, demandando il caricamento (e la gestione di eventuali errori) a sistemi terzi</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_CDA2_RAD_CT5_KO</t>
   </si>
   <si>
@@ -592,6 +591,12 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>5e02c58c47986639</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50504.4.4.930de4356d88c2c4150942eac66d3ef84e9b237be1c5ed78390cc9e0426578ff.1340451039^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
@@ -784,7 +789,7 @@
   <fonts count="6">
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -794,7 +799,6 @@
     <font>
       <b/>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -806,14 +810,12 @@
     <font>
       <b/>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <u/>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1021,7 +1023,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1122,6 +1124,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="9" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
@@ -1146,10 +1152,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
@@ -1158,27 +1160,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1222,7 +1212,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{979658E4-2E59-97D9-C944-5EC786B05672}"/>
+  <person displayName=" " id="{160E8926-4277-9515-DB2E-1F6573C4200C}"/>
 </personList>
 </file>
 
@@ -1698,7 +1688,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E9" personId="{979658E4-2E59-97D9-C944-5EC786B05672}" id="{00040094-0080-4043-9688-008D000D00A7}" done="0">
+  <threadedComment ref="E9" personId="{160E8926-4277-9515-DB2E-1F6573C4200C}" id="{00040094-0080-4043-9688-008D000D00A7}" done="0">
     <text xml:space="preserve">======
 ID#AAAAzAuRGEo
     (2023-06-14 09:12:48)
@@ -3906,8 +3896,8 @@
     <col customWidth="1" min="5" max="5" style="0" width="23.219999999999999"/>
     <col customWidth="1" min="6" max="6" style="0" width="11.710000000000001"/>
     <col customWidth="1" min="7" max="7" style="0" width="12.42"/>
-    <col customWidth="1" min="8" max="8" style="0" width="14"/>
-    <col customWidth="1" min="9" max="9" style="0" width="14.58"/>
+    <col customWidth="1" min="8" max="8" style="0" width="19.28125"/>
+    <col customWidth="1" min="9" max="9" style="0" width="150.8515625"/>
     <col customWidth="1" min="10" max="10" style="0" width="27.149999999999999"/>
     <col customWidth="1" min="11" max="15" style="0" width="36.43"/>
     <col customWidth="1" min="16" max="16" style="0" width="27.149999999999999"/>
@@ -4086,7 +4076,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="13"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" ht="56.25">
       <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
@@ -4164,26 +4154,34 @@
       <c r="E10" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="27" t="s">
+      <c r="F10" s="25">
+        <v>45126</v>
+      </c>
+      <c r="G10" s="26">
+        <v>0.49715277777777778</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="28" t="s">
+      <c r="I10" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="S10" s="29"/>
-      <c r="T10" s="30" t="s">
+      <c r="J10" s="28" t="s">
         <v>53</v>
+      </c>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="S10" s="30"/>
+      <c r="T10" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -4197,33 +4195,33 @@
         <v>48</v>
       </c>
       <c r="D11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="25"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="K11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="S11" s="30"/>
+      <c r="T11" s="31" t="s">
         <v>55</v>
-      </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="S11" s="29"/>
-      <c r="T11" s="30" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
@@ -4237,33 +4235,33 @@
         <v>48</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E12" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="25"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
       <c r="R12" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S12" s="29"/>
-      <c r="T12" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="S12" s="30"/>
+      <c r="T12" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
@@ -4277,33 +4275,33 @@
         <v>48</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27" t="s">
-        <v>52</v>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="K13" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
+        <v>58</v>
+      </c>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
       <c r="R13" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S13" s="29"/>
-      <c r="T13" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="S13" s="30"/>
+      <c r="T13" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -4317,33 +4315,33 @@
         <v>48</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K14" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
       <c r="R14" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S14" s="29"/>
-      <c r="T14" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S14" s="30"/>
+      <c r="T14" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
@@ -4357,33 +4355,33 @@
         <v>48</v>
       </c>
       <c r="D15" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="S15" s="30"/>
+      <c r="T15" s="31" t="s">
         <v>66</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="K15" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S15" s="29"/>
-      <c r="T15" s="30" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -4397,33 +4395,43 @@
         <v>48</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O16" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q16" s="28"/>
       <c r="R16" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S16" s="29"/>
-      <c r="T16" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S16" s="30"/>
+      <c r="T16" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -4437,33 +4445,33 @@
         <v>48</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="28"/>
       <c r="R17" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S17" s="29"/>
-      <c r="T17" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S17" s="30"/>
+      <c r="T17" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
@@ -4477,33 +4485,33 @@
         <v>48</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27" t="s">
-        <v>52</v>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
+        <v>78</v>
+      </c>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
       <c r="R18" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S18" s="29"/>
-      <c r="T18" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S18" s="30"/>
+      <c r="T18" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
@@ -4517,33 +4525,33 @@
         <v>48</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
       <c r="R19" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S19" s="29"/>
-      <c r="T19" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S19" s="30"/>
+      <c r="T19" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -4557,33 +4565,33 @@
         <v>48</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>83</v>
       </c>
       <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K20" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
       <c r="R20" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S20" s="29"/>
-      <c r="T20" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S20" s="30"/>
+      <c r="T20" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
@@ -4597,33 +4605,33 @@
         <v>48</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27" t="s">
-        <v>52</v>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
+        <v>75</v>
+      </c>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
       <c r="R21" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S21" s="29"/>
-      <c r="T21" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S21" s="30"/>
+      <c r="T21" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
@@ -4637,33 +4645,33 @@
         <v>48</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
       <c r="R22" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S22" s="29"/>
-      <c r="T22" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S22" s="30"/>
+      <c r="T22" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -4677,33 +4685,33 @@
         <v>48</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K23" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
       <c r="R23" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S23" s="29"/>
-      <c r="T23" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S23" s="30"/>
+      <c r="T23" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
@@ -4717,33 +4725,33 @@
         <v>48</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K24" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
       <c r="R24" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S24" s="29"/>
-      <c r="T24" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S24" s="30"/>
+      <c r="T24" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
@@ -4757,33 +4765,33 @@
         <v>48</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27" t="s">
-        <v>52</v>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
+        <v>75</v>
+      </c>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
       <c r="R25" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S25" s="29"/>
-      <c r="T25" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S25" s="30"/>
+      <c r="T25" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -4797,33 +4805,33 @@
         <v>48</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K26" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
       <c r="R26" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S26" s="29"/>
-      <c r="T26" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S26" s="30"/>
+      <c r="T26" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
@@ -4837,33 +4845,33 @@
         <v>48</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K27" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
       <c r="R27" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S27" s="29"/>
-      <c r="T27" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S27" s="30"/>
+      <c r="T27" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
@@ -4877,33 +4885,33 @@
         <v>48</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K28" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
       <c r="R28" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S28" s="29"/>
-      <c r="T28" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S28" s="30"/>
+      <c r="T28" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -4917,33 +4925,33 @@
         <v>48</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K29" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
       <c r="R29" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S29" s="29"/>
-      <c r="T29" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S29" s="30"/>
+      <c r="T29" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
@@ -4957,33 +4965,33 @@
         <v>48</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K30" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
       <c r="R30" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S30" s="29"/>
-      <c r="T30" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S30" s="30"/>
+      <c r="T30" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
@@ -4997,33 +5005,33 @@
         <v>48</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K31" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
       <c r="R31" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S31" s="29"/>
-      <c r="T31" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S31" s="30"/>
+      <c r="T31" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -5037,33 +5045,33 @@
         <v>48</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K32" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
       <c r="R32" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S32" s="29"/>
-      <c r="T32" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S32" s="30"/>
+      <c r="T32" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
@@ -5077,33 +5085,33 @@
         <v>48</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K33" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
       <c r="R33" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S33" s="29"/>
-      <c r="T33" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S33" s="30"/>
+      <c r="T33" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
@@ -5117,33 +5125,33 @@
         <v>48</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K34" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L34" s="27"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K34" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
       <c r="R34" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="S34" s="29"/>
-      <c r="T34" s="30" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S34" s="30"/>
+      <c r="T34" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -5157,33 +5165,33 @@
         <v>48</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="K35" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="S35" s="29"/>
-      <c r="T35" s="30" t="s">
-        <v>64</v>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="S35" s="30"/>
+      <c r="T35" s="31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
@@ -5197,31 +5205,39 @@
         <v>48</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
-      <c r="R36" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="S36" s="29"/>
-      <c r="T36" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="25">
+        <v>45126</v>
+      </c>
+      <c r="G36" s="26">
+        <v>0.49942129629629628</v>
+      </c>
+      <c r="H36" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36" s="28" t="s">
         <v>53</v>
+      </c>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="S36" s="30"/>
+      <c r="T36" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
@@ -9894,7 +9910,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D90030-0052-4BBB-BF75-005C003A0063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00F20037-00B8-4780-A386-00EC006D004D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
@@ -9903,7 +9919,7 @@
           </x14:formula2>
           <xm:sqref>J10:J36 L10:M36 O10:O36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B0008A-0057-4305-BB28-002000790093}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{002000E7-0077-424A-BE78-007D009000B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -9947,38 +9963,38 @@
         <v>28</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
@@ -9986,125 +10002,125 @@
         <v>48</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="43" t="s">
-        <v>126</v>
+      <c r="C4" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>132</v>
+        <v>125</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="7" ht="15">
       <c r="A7" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="8" ht="15">
       <c r="A8" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>138</v>
+        <v>125</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="9" ht="15">
       <c r="A9" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>141</v>
+        <v>125</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" ht="42.75">
       <c r="A10" s="10" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>144</v>
+        <v>125</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="42">
+        <v>151</v>
+      </c>
+      <c r="C11" s="39">
         <v>192</v>
       </c>
-      <c r="D11" s="42" t="s">
-        <v>146</v>
+      <c r="D11" s="39" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" s="42">
+        <v>151</v>
+      </c>
+      <c r="C12" s="39">
         <v>208</v>
       </c>
-      <c r="D12" s="42" t="s">
-        <v>147</v>
+      <c r="D12" s="39" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
@@ -10112,111 +10128,111 @@
         <v>48</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="42">
+        <v>151</v>
+      </c>
+      <c r="C13" s="39">
         <v>224</v>
       </c>
-      <c r="D13" s="43" t="s">
-        <v>148</v>
+      <c r="D13" s="40" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C14" s="42">
+        <v>151</v>
+      </c>
+      <c r="C14" s="39">
         <v>240</v>
       </c>
-      <c r="D14" s="42" t="s">
-        <v>149</v>
+      <c r="D14" s="39" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C15" s="42">
+        <v>151</v>
+      </c>
+      <c r="C15" s="39">
         <v>256</v>
       </c>
-      <c r="D15" s="43" t="s">
-        <v>150</v>
+      <c r="D15" s="40" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C16" s="42">
+        <v>151</v>
+      </c>
+      <c r="C16" s="39">
         <v>272</v>
       </c>
-      <c r="D16" s="43" t="s">
-        <v>151</v>
+      <c r="D16" s="40" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="42">
+        <v>151</v>
+      </c>
+      <c r="C17" s="39">
         <v>288</v>
       </c>
-      <c r="D17" s="43" t="s">
-        <v>152</v>
+      <c r="D17" s="40" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="42">
+        <v>151</v>
+      </c>
+      <c r="C18" s="39">
         <v>304</v>
       </c>
-      <c r="D18" s="43" t="s">
-        <v>153</v>
+      <c r="D18" s="40" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="42">
+        <v>160</v>
+      </c>
+      <c r="C19" s="39">
         <v>193</v>
       </c>
-      <c r="D19" s="42" t="s">
-        <v>155</v>
+      <c r="D19" s="39" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" s="42">
+        <v>160</v>
+      </c>
+      <c r="C20" s="39">
         <v>209</v>
       </c>
-      <c r="D20" s="42" t="s">
-        <v>156</v>
+      <c r="D20" s="39" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
@@ -10224,111 +10240,111 @@
         <v>48</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="42">
+        <v>160</v>
+      </c>
+      <c r="C21" s="39">
         <v>225</v>
       </c>
-      <c r="D21" s="43" t="s">
-        <v>157</v>
+      <c r="D21" s="40" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="42">
+        <v>160</v>
+      </c>
+      <c r="C22" s="39">
         <v>241</v>
       </c>
-      <c r="D22" s="42" t="s">
-        <v>158</v>
+      <c r="D22" s="39" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" s="42">
+        <v>160</v>
+      </c>
+      <c r="C23" s="39">
         <v>257</v>
       </c>
-      <c r="D23" s="43" t="s">
-        <v>159</v>
+      <c r="D23" s="40" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C24" s="42">
+        <v>160</v>
+      </c>
+      <c r="C24" s="39">
         <v>273</v>
       </c>
-      <c r="D24" s="43" t="s">
-        <v>160</v>
+      <c r="D24" s="40" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="42">
+        <v>160</v>
+      </c>
+      <c r="C25" s="39">
         <v>289</v>
       </c>
-      <c r="D25" s="43" t="s">
-        <v>161</v>
+      <c r="D25" s="40" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C26" s="42">
+        <v>160</v>
+      </c>
+      <c r="C26" s="39">
         <v>305</v>
       </c>
-      <c r="D26" s="43" t="s">
-        <v>162</v>
+      <c r="D26" s="40" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="42">
+        <v>169</v>
+      </c>
+      <c r="C27" s="39">
         <v>194</v>
       </c>
-      <c r="D27" s="42" t="s">
-        <v>164</v>
+      <c r="D27" s="39" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C28" s="42">
+        <v>169</v>
+      </c>
+      <c r="C28" s="39">
         <v>210</v>
       </c>
-      <c r="D28" s="42" t="s">
-        <v>165</v>
+      <c r="D28" s="39" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -10336,110 +10352,110 @@
         <v>48</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C29" s="42">
+        <v>169</v>
+      </c>
+      <c r="C29" s="39">
         <v>226</v>
       </c>
-      <c r="D29" s="44" t="s">
-        <v>166</v>
+      <c r="D29" s="41" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="42">
+        <v>169</v>
+      </c>
+      <c r="C30" s="39">
         <v>242</v>
       </c>
-      <c r="D30" s="42" t="s">
-        <v>167</v>
+      <c r="D30" s="39" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C31" s="42">
+        <v>169</v>
+      </c>
+      <c r="C31" s="39">
         <v>258</v>
       </c>
-      <c r="D31" s="43" t="s">
-        <v>168</v>
+      <c r="D31" s="40" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C32" s="42">
+        <v>169</v>
+      </c>
+      <c r="C32" s="39">
         <v>274</v>
       </c>
-      <c r="D32" s="43" t="s">
-        <v>169</v>
+      <c r="D32" s="40" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="42">
+        <v>169</v>
+      </c>
+      <c r="C33" s="39">
         <v>290</v>
       </c>
-      <c r="D33" s="43" t="s">
-        <v>170</v>
+      <c r="D33" s="40" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="42">
+        <v>169</v>
+      </c>
+      <c r="C34" s="39">
         <v>306</v>
       </c>
-      <c r="D34" s="43" t="s">
-        <v>171</v>
+      <c r="D34" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="42">
+        <v>178</v>
+      </c>
+      <c r="C35" s="39">
         <v>195</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="39">
         <v>204</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C36" s="42">
+        <v>178</v>
+      </c>
+      <c r="C36" s="39">
         <v>211</v>
       </c>
-      <c r="D36" s="42">
+      <c r="D36" s="39">
         <v>220</v>
       </c>
     </row>
@@ -10448,110 +10464,110 @@
         <v>48</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C37" s="42">
+        <v>178</v>
+      </c>
+      <c r="C37" s="39">
         <v>227</v>
       </c>
-      <c r="D37" s="43">
+      <c r="D37" s="40">
         <v>236</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C38" s="42">
+        <v>178</v>
+      </c>
+      <c r="C38" s="39">
         <v>243</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="39">
         <v>252</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C39" s="42">
+        <v>178</v>
+      </c>
+      <c r="C39" s="39">
         <v>259</v>
       </c>
-      <c r="D39" s="43">
+      <c r="D39" s="40">
         <v>268</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="42">
+        <v>178</v>
+      </c>
+      <c r="C40" s="39">
         <v>275</v>
       </c>
-      <c r="D40" s="43">
+      <c r="D40" s="40">
         <v>284</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C41" s="42">
+        <v>178</v>
+      </c>
+      <c r="C41" s="39">
         <v>291</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="40">
         <v>300</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C42" s="42">
+        <v>178</v>
+      </c>
+      <c r="C42" s="39">
         <v>307</v>
       </c>
-      <c r="D42" s="43">
+      <c r="D42" s="40">
         <v>316</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C43" s="42">
+        <v>179</v>
+      </c>
+      <c r="C43" s="39">
         <v>196</v>
       </c>
-      <c r="D43" s="42">
+      <c r="D43" s="39">
         <v>207</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C44" s="42">
+        <v>179</v>
+      </c>
+      <c r="C44" s="39">
         <v>212</v>
       </c>
-      <c r="D44" s="42">
+      <c r="D44" s="39">
         <v>223</v>
       </c>
     </row>
@@ -10560,82 +10576,82 @@
         <v>48</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C45" s="42">
+        <v>179</v>
+      </c>
+      <c r="C45" s="39">
         <v>228</v>
       </c>
-      <c r="D45" s="43">
+      <c r="D45" s="40">
         <v>239</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" s="42">
+        <v>179</v>
+      </c>
+      <c r="C46" s="39">
         <v>244</v>
       </c>
-      <c r="D46" s="42">
+      <c r="D46" s="39">
         <v>255</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" s="42">
+        <v>179</v>
+      </c>
+      <c r="C47" s="39">
         <v>260</v>
       </c>
-      <c r="D47" s="43">
+      <c r="D47" s="40">
         <v>271</v>
       </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C48" s="42">
+        <v>179</v>
+      </c>
+      <c r="C48" s="39">
         <v>276</v>
       </c>
-      <c r="D48" s="43">
+      <c r="D48" s="40">
         <v>287</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C49" s="42">
+        <v>179</v>
+      </c>
+      <c r="C49" s="39">
         <v>292</v>
       </c>
-      <c r="D49" s="43">
+      <c r="D49" s="40">
         <v>303</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C50" s="42">
+        <v>179</v>
+      </c>
+      <c r="C50" s="39">
         <v>308</v>
       </c>
-      <c r="D50" s="43">
+      <c r="D50" s="40">
         <v>319</v>
       </c>
     </row>
@@ -11616,32 +11632,32 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="42" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>51</v>
+      <c r="A2" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>52</v>
+      <c r="A3" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
     <row r="6" ht="14.25" customHeight="1"/>

</xml_diff>